<commit_message>
add 2nd ATPase reaction, remove ADK
</commit_message>
<xml_diff>
--- a/metabolite_data/lt_dataset2_quantified.xlsx
+++ b/metabolite_data/lt_dataset2_quantified.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\Lynd Lab research\Ctherm CBP project\thermodynamic analysis with Satya 11-30-2018\Ctherm_thermo\metabolite_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/satyakam/Dropbox/Work/component_contribution_ctherm/metabolite_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BBE378-5395-4331-BE5A-2BDF818EB2BA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -265,7 +272,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -386,9 +393,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -416,31 +423,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -468,23 +458,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -660,16 +633,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="I260" sqref="I260"/>
+    <sheetView tabSelected="1" topLeftCell="C250" workbookViewId="0">
+      <selection activeCell="O255" sqref="O255:O266"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -772,7 +745,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -825,7 +798,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -878,7 +851,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -931,7 +904,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -984,7 +957,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1037,7 +1010,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1090,7 +1063,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1143,7 +1116,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1196,7 +1169,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1249,7 +1222,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1302,7 +1275,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1355,7 +1328,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1408,7 +1381,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1461,7 +1434,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1514,7 +1487,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1567,7 +1540,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1620,7 +1593,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1673,7 +1646,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1726,7 +1699,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1779,7 +1752,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1832,7 +1805,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1885,7 +1858,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1938,7 +1911,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1991,7 +1964,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2044,7 +2017,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2097,7 +2070,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2150,7 +2123,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2203,7 +2176,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2256,7 +2229,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2309,7 +2282,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2362,7 +2335,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2415,7 +2388,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2468,7 +2441,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2521,7 +2494,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2574,7 +2547,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2627,7 +2600,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2680,7 +2653,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2733,7 +2706,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2786,7 +2759,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2839,7 +2812,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2892,7 +2865,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2945,7 +2918,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2998,7 +2971,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3051,7 +3024,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3104,7 +3077,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3157,7 +3130,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3210,7 +3183,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3263,7 +3236,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3316,7 +3289,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3369,7 +3342,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3422,7 +3395,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3475,7 +3448,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3528,7 +3501,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3581,7 +3554,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3634,7 +3607,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3687,7 +3660,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3740,7 +3713,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3793,7 +3766,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3846,7 +3819,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3899,7 +3872,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3952,7 +3925,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4005,7 +3978,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -4058,7 +4031,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -4111,7 +4084,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -4164,7 +4137,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -4217,7 +4190,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -4270,7 +4243,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4323,7 +4296,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -4376,7 +4349,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -4429,7 +4402,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -4482,7 +4455,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -4535,7 +4508,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -4588,7 +4561,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -4641,7 +4614,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -4694,7 +4667,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -4747,7 +4720,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -4800,7 +4773,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -4853,7 +4826,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4906,7 +4879,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4959,7 +4932,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -5012,7 +4985,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -5065,7 +5038,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -5118,7 +5091,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -5171,7 +5144,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -5224,7 +5197,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -5277,7 +5250,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -5330,7 +5303,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -5383,7 +5356,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -5436,7 +5409,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -5489,7 +5462,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -5542,7 +5515,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -5595,7 +5568,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -5648,7 +5621,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -5701,7 +5674,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -5754,7 +5727,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -5807,7 +5780,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -5860,7 +5833,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -5913,7 +5886,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -5966,7 +5939,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -6019,7 +5992,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -6072,7 +6045,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -6125,7 +6098,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -6178,7 +6151,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -6231,7 +6204,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -6284,7 +6257,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -6337,7 +6310,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -6390,7 +6363,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -6443,7 +6416,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -6496,7 +6469,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -6549,7 +6522,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -6602,7 +6575,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -6655,7 +6628,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -6708,7 +6681,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -6761,7 +6734,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -6814,7 +6787,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -6867,7 +6840,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -6920,7 +6893,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -6973,7 +6946,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -7026,7 +6999,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -7079,7 +7052,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -7132,7 +7105,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -7185,7 +7158,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -7238,7 +7211,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -7291,7 +7264,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -7344,7 +7317,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -7397,7 +7370,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -7450,7 +7423,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -7503,7 +7476,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -7556,7 +7529,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -7609,7 +7582,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -7662,7 +7635,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -7715,7 +7688,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -7768,7 +7741,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -7821,7 +7794,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -7874,7 +7847,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -7927,7 +7900,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -7980,7 +7953,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -8033,7 +8006,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -8086,7 +8059,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -8139,7 +8112,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -8192,7 +8165,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -8245,7 +8218,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -8298,7 +8271,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -8351,7 +8324,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -8404,7 +8377,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -8457,7 +8430,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -8510,7 +8483,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -8563,7 +8536,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -8616,7 +8589,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -8669,7 +8642,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -8722,7 +8695,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -8775,7 +8748,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -8828,7 +8801,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -8881,7 +8854,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -8934,7 +8907,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -8987,7 +8960,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -9040,7 +9013,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -9093,7 +9066,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -9146,7 +9119,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -9199,7 +9172,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -9252,7 +9225,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -9305,7 +9278,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -9358,7 +9331,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -9411,7 +9384,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -9464,7 +9437,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -9517,7 +9490,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -9570,7 +9543,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -9623,7 +9596,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -9676,7 +9649,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -9729,7 +9702,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -9782,7 +9755,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -9835,7 +9808,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -9888,7 +9861,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -9941,7 +9914,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -9994,7 +9967,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -10047,7 +10020,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -10100,7 +10073,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -10153,7 +10126,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -10206,7 +10179,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -10259,7 +10232,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -10312,7 +10285,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -10365,7 +10338,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -10418,7 +10391,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -10471,7 +10444,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -10524,7 +10497,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -10577,7 +10550,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -10630,7 +10603,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -10683,7 +10656,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -10736,7 +10709,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -10789,7 +10762,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -10842,7 +10815,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -10895,7 +10868,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -10948,7 +10921,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -11001,7 +10974,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -11054,7 +11027,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -11107,7 +11080,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -11160,7 +11133,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -11213,7 +11186,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -11266,7 +11239,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -11319,7 +11292,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -11372,7 +11345,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -11425,7 +11398,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -11478,7 +11451,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -11531,7 +11504,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -11584,7 +11557,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -11637,7 +11610,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -11690,7 +11663,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -11743,7 +11716,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -11796,7 +11769,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -11849,7 +11822,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -11902,7 +11875,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -11955,7 +11928,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -12008,7 +11981,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -12061,7 +12034,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -12114,7 +12087,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -12167,7 +12140,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -12220,7 +12193,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -12273,7 +12246,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -12326,7 +12299,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -12379,7 +12352,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -12432,7 +12405,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -12485,7 +12458,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -12538,7 +12511,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -12591,7 +12564,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -12644,7 +12617,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -12697,7 +12670,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -12750,7 +12723,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -12803,7 +12776,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -12856,7 +12829,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -12909,7 +12882,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -12962,7 +12935,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -13015,7 +12988,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -13068,7 +13041,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -13121,7 +13094,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -13174,7 +13147,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -13227,7 +13200,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -13280,7 +13253,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -13333,7 +13306,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -13386,7 +13359,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -13439,7 +13412,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -13492,7 +13465,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -13545,7 +13518,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -13598,7 +13571,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -13651,7 +13624,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -13704,7 +13677,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -13757,7 +13730,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -13810,7 +13783,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -13863,7 +13836,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -13916,7 +13889,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -13969,7 +13942,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -14022,7 +13995,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -14075,7 +14048,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -14128,7 +14101,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>0</v>
       </c>
@@ -14156,6 +14129,10 @@
       <c r="M255" t="s">
         <v>55</v>
       </c>
+      <c r="O255">
+        <f>I255/46</f>
+        <v>0.11130434782608696</v>
+      </c>
       <c r="P255">
         <v>108530.4970696766</v>
       </c>
@@ -14163,7 +14140,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>1</v>
       </c>
@@ -14191,6 +14168,10 @@
       <c r="M256" t="s">
         <v>55</v>
       </c>
+      <c r="O256">
+        <f t="shared" ref="O256:O266" si="0">I256/46</f>
+        <v>0.11130434782608696</v>
+      </c>
       <c r="P256">
         <v>108530.4970696766</v>
       </c>
@@ -14198,7 +14179,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>2</v>
       </c>
@@ -14226,6 +14207,10 @@
       <c r="M257" t="s">
         <v>55</v>
       </c>
+      <c r="O257">
+        <f t="shared" si="0"/>
+        <v>0.43934782608695655</v>
+      </c>
       <c r="P257">
         <v>434121.98827870633</v>
       </c>
@@ -14233,7 +14218,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>3</v>
       </c>
@@ -14261,6 +14246,10 @@
       <c r="M258" t="s">
         <v>55</v>
       </c>
+      <c r="O258">
+        <f t="shared" si="0"/>
+        <v>0.43934782608695655</v>
+      </c>
       <c r="P258">
         <v>434121.98827870633</v>
       </c>
@@ -14268,7 +14257,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>4</v>
       </c>
@@ -14296,6 +14285,10 @@
       <c r="M259" t="s">
         <v>55</v>
       </c>
+      <c r="O259">
+        <f t="shared" si="0"/>
+        <v>0.87782608695652176</v>
+      </c>
       <c r="P259">
         <v>868243.97655741253</v>
       </c>
@@ -14303,7 +14296,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>5</v>
       </c>
@@ -14331,6 +14324,10 @@
       <c r="M260" t="s">
         <v>55</v>
       </c>
+      <c r="O260">
+        <f t="shared" si="0"/>
+        <v>0.87782608695652176</v>
+      </c>
       <c r="P260">
         <v>868243.97655741253</v>
       </c>
@@ -14338,7 +14335,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>6</v>
       </c>
@@ -14366,6 +14363,10 @@
       <c r="M261" t="s">
         <v>55</v>
       </c>
+      <c r="O261">
+        <f t="shared" si="0"/>
+        <v>4.3478260869565218E-3</v>
+      </c>
       <c r="P261">
         <v>4341.2198827870634</v>
       </c>
@@ -14373,7 +14374,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>7</v>
       </c>
@@ -14401,6 +14402,10 @@
       <c r="M262" t="s">
         <v>55</v>
       </c>
+      <c r="O262">
+        <f t="shared" si="0"/>
+        <v>4.3478260869565218E-3</v>
+      </c>
       <c r="P262">
         <v>4341.2198827870634</v>
       </c>
@@ -14408,7 +14413,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>8</v>
       </c>
@@ -14436,6 +14441,10 @@
       <c r="M263" t="s">
         <v>55</v>
       </c>
+      <c r="O263">
+        <f t="shared" si="0"/>
+        <v>1.0217391304347826E-2</v>
+      </c>
       <c r="P263">
         <v>10201.8667245496</v>
       </c>
@@ -14443,7 +14452,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>9</v>
       </c>
@@ -14471,6 +14480,10 @@
       <c r="M264" t="s">
         <v>55</v>
       </c>
+      <c r="O264">
+        <f t="shared" si="0"/>
+        <v>1.0217391304347826E-2</v>
+      </c>
       <c r="P264">
         <v>10201.8667245496</v>
       </c>
@@ -14478,7 +14491,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>10</v>
       </c>
@@ -14506,6 +14519,10 @@
       <c r="M265" t="s">
         <v>55</v>
       </c>
+      <c r="O265">
+        <f t="shared" si="0"/>
+        <v>1.2608695652173912E-2</v>
+      </c>
       <c r="P265">
         <v>12589.53766008248</v>
       </c>
@@ -14513,7 +14530,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>11</v>
       </c>
@@ -14540,6 +14557,10 @@
       </c>
       <c r="M266" t="s">
         <v>55</v>
+      </c>
+      <c r="O266">
+        <f t="shared" si="0"/>
+        <v>1.2608695652173912E-2</v>
       </c>
       <c r="P266">
         <v>12589.53766008248</v>

</xml_diff>